<commit_message>
Update PSR_전원 L100 케이블_12_35 20240724_2.xlsx
</commit_message>
<xml_diff>
--- a/PSR_전원 L100 케이블_12_35 20240724_2.xlsx
+++ b/PSR_전원 L100 케이블_12_35 20240724_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twinpapa/Library/Mobile Documents/com~apple~CloudDocs/JDS_Data/NEW_Pro/홍콩_AS/이슈사항/제작도/240528_최종확인/하네스 및 조립방법/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/JDS_BU/Git_Hub/GIC_HONGKONG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C5C10D2-A7FC-ED4E-9A19-CA4048B816DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84B854C-6D5A-2D44-A4F6-DC0314CE2DB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="41120" windowHeight="24840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CABLE ASS'Y" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
   <si>
     <t>Pin map</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -231,6 +231,10 @@
   </si>
   <si>
     <t>0.5 -&gt; 1.0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>dddddd</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -856,6 +860,84 @@
     <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -863,112 +945,34 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="20" fillId="7" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1760,10 +1764,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q41"/>
+  <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36:K36"/>
+      <selection activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="17" outlineLevelRow="1"/>
@@ -1787,22 +1791,22 @@
   <sheetData>
     <row r="1" spans="1:16" ht="22">
       <c r="A1" s="35"/>
-      <c r="B1" s="74" t="s">
+      <c r="B1" s="102" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
-      <c r="L1" s="74"/>
-      <c r="M1" s="74"/>
-      <c r="N1" s="74"/>
-      <c r="O1" s="74"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="102"/>
+      <c r="E1" s="102"/>
+      <c r="F1" s="102"/>
+      <c r="G1" s="102"/>
+      <c r="H1" s="102"/>
+      <c r="I1" s="102"/>
+      <c r="J1" s="102"/>
+      <c r="K1" s="102"/>
+      <c r="L1" s="102"/>
+      <c r="M1" s="102"/>
+      <c r="N1" s="102"/>
+      <c r="O1" s="102"/>
       <c r="P1" s="1"/>
     </row>
     <row r="2" spans="1:16" outlineLevel="1">
@@ -1824,28 +1828,28 @@
       <c r="C4" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="75" t="s">
+      <c r="D4" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="75"/>
+      <c r="E4" s="86"/>
       <c r="F4" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="75" t="s">
+      <c r="G4" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="86"/>
       <c r="J4" s="29" t="s">
         <v>6</v>
       </c>
       <c r="K4" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="75" t="s">
+      <c r="L4" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="M4" s="75"/>
+      <c r="M4" s="86"/>
       <c r="N4" s="29" t="s">
         <v>2</v>
       </c>
@@ -1856,93 +1860,93 @@
     </row>
     <row r="5" spans="1:16" ht="16.5" customHeight="1" outlineLevel="1">
       <c r="A5" s="36"/>
-      <c r="B5" s="76" t="s">
+      <c r="B5" s="103" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="80" t="s">
+      <c r="C5" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="78" t="s">
+      <c r="D5" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="78"/>
+      <c r="E5" s="72"/>
       <c r="F5" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="G5" s="103" t="s">
+      <c r="G5" s="104" t="s">
         <v>45</v>
       </c>
-      <c r="H5" s="103"/>
-      <c r="I5" s="103"/>
+      <c r="H5" s="104"/>
+      <c r="I5" s="104"/>
       <c r="J5" s="61" t="s">
         <v>25</v>
       </c>
       <c r="K5" s="60"/>
-      <c r="L5" s="78">
+      <c r="L5" s="72">
         <v>1</v>
       </c>
-      <c r="M5" s="78"/>
-      <c r="N5" s="78" t="s">
+      <c r="M5" s="72"/>
+      <c r="N5" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="O5" s="79" t="s">
+      <c r="O5" s="76" t="s">
         <v>32</v>
       </c>
       <c r="P5" s="5"/>
     </row>
     <row r="6" spans="1:16" ht="16.5" customHeight="1" outlineLevel="1">
       <c r="A6" s="36"/>
-      <c r="B6" s="76"/>
-      <c r="C6" s="81"/>
-      <c r="D6" s="78" t="s">
+      <c r="B6" s="103"/>
+      <c r="C6" s="88"/>
+      <c r="D6" s="72" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="78"/>
+      <c r="E6" s="72"/>
       <c r="F6" s="60"/>
-      <c r="G6" s="77" t="s">
+      <c r="G6" s="97" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="77"/>
-      <c r="I6" s="77"/>
+      <c r="H6" s="97"/>
+      <c r="I6" s="97"/>
       <c r="J6" s="61" t="s">
         <v>20</v>
       </c>
       <c r="K6" s="60"/>
-      <c r="L6" s="78">
+      <c r="L6" s="72">
         <v>5</v>
       </c>
-      <c r="M6" s="78"/>
-      <c r="N6" s="78"/>
-      <c r="O6" s="79"/>
+      <c r="M6" s="72"/>
+      <c r="N6" s="72"/>
+      <c r="O6" s="76"/>
       <c r="P6" s="5"/>
     </row>
     <row r="7" spans="1:16" ht="16.5" customHeight="1" outlineLevel="1">
       <c r="A7" s="36"/>
-      <c r="B7" s="76"/>
-      <c r="C7" s="82"/>
-      <c r="D7" s="78" t="s">
+      <c r="B7" s="103"/>
+      <c r="C7" s="89"/>
+      <c r="D7" s="72" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="78"/>
+      <c r="E7" s="72"/>
       <c r="F7" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="103" t="s">
+      <c r="G7" s="104" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="103"/>
-      <c r="I7" s="103"/>
+      <c r="H7" s="104"/>
+      <c r="I7" s="104"/>
       <c r="J7" s="61" t="str">
         <f>J5</f>
         <v>100mm</v>
       </c>
       <c r="K7" s="60"/>
-      <c r="L7" s="78">
+      <c r="L7" s="72">
         <v>3</v>
       </c>
-      <c r="M7" s="78"/>
-      <c r="N7" s="78"/>
-      <c r="O7" s="79"/>
+      <c r="M7" s="72"/>
+      <c r="N7" s="72"/>
+      <c r="O7" s="76"/>
       <c r="P7" s="5"/>
     </row>
     <row r="8" spans="1:16">
@@ -1958,10 +1962,10 @@
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="99"/>
-      <c r="H9" s="99"/>
-      <c r="I9" s="99"/>
-      <c r="J9" s="99"/>
+      <c r="G9" s="98"/>
+      <c r="H9" s="98"/>
+      <c r="I9" s="98"/>
+      <c r="J9" s="98"/>
       <c r="K9" s="3"/>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
@@ -1973,22 +1977,22 @@
       <c r="A10" s="36"/>
       <c r="B10" s="16"/>
       <c r="C10" s="3"/>
-      <c r="D10" s="88" t="str">
+      <c r="D10" s="80" t="str">
         <f>B5</f>
         <v>WAGO
 770-173</v>
       </c>
       <c r="E10" s="31"/>
       <c r="F10" s="62"/>
-      <c r="G10" s="91"/>
-      <c r="H10" s="94" t="s">
+      <c r="G10" s="83"/>
+      <c r="H10" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="I10" s="94"/>
-      <c r="J10" s="85"/>
+      <c r="I10" s="67"/>
+      <c r="J10" s="90"/>
       <c r="K10" s="63"/>
       <c r="L10" s="10"/>
-      <c r="M10" s="67" t="str">
+      <c r="M10" s="93" t="str">
         <f>O5</f>
         <v>YEONHO
 YH396-05V</v>
@@ -2001,7 +2005,7 @@
       <c r="A11" s="36"/>
       <c r="B11" s="16"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="89"/>
+      <c r="D11" s="81"/>
       <c r="E11" s="32" t="s">
         <v>28</v>
       </c>
@@ -2009,42 +2013,42 @@
         <f>F5</f>
         <v>L/DC 110V / CON1-Vin+</v>
       </c>
-      <c r="G11" s="92"/>
-      <c r="H11" s="95"/>
-      <c r="I11" s="95"/>
-      <c r="J11" s="86"/>
+      <c r="G11" s="84"/>
+      <c r="H11" s="68"/>
+      <c r="I11" s="68"/>
+      <c r="J11" s="91"/>
       <c r="K11" s="64"/>
       <c r="L11" s="66">
         <v>1</v>
       </c>
-      <c r="M11" s="68"/>
+      <c r="M11" s="94"/>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
       <c r="P11" s="9"/>
     </row>
     <row r="12" spans="1:16" s="8" customFormat="1" ht="16.5" customHeight="1">
       <c r="A12" s="36"/>
-      <c r="B12" s="70"/>
-      <c r="C12" s="71"/>
-      <c r="D12" s="89"/>
+      <c r="B12" s="100"/>
+      <c r="C12" s="101"/>
+      <c r="D12" s="81"/>
       <c r="E12" s="32"/>
       <c r="F12" s="64"/>
-      <c r="G12" s="92"/>
-      <c r="H12" s="95"/>
-      <c r="I12" s="95"/>
-      <c r="J12" s="86"/>
+      <c r="G12" s="84"/>
+      <c r="H12" s="68"/>
+      <c r="I12" s="68"/>
+      <c r="J12" s="91"/>
       <c r="K12" s="64"/>
       <c r="L12" s="34"/>
-      <c r="M12" s="68"/>
+      <c r="M12" s="94"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
       <c r="P12" s="9"/>
     </row>
     <row r="13" spans="1:16" s="8" customFormat="1" ht="16.5" customHeight="1">
       <c r="A13" s="36"/>
-      <c r="B13" s="70"/>
-      <c r="C13" s="71"/>
-      <c r="D13" s="89"/>
+      <c r="B13" s="100"/>
+      <c r="C13" s="101"/>
+      <c r="D13" s="81"/>
       <c r="E13" s="32" t="s">
         <v>30</v>
       </c>
@@ -2052,15 +2056,15 @@
         <f>F7</f>
         <v>N/DC GND / CON1-Vin-</v>
       </c>
-      <c r="G13" s="92"/>
-      <c r="H13" s="95"/>
-      <c r="I13" s="95"/>
-      <c r="J13" s="86"/>
+      <c r="G13" s="84"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="68"/>
+      <c r="J13" s="91"/>
       <c r="K13" s="64"/>
       <c r="L13" s="34">
         <v>3</v>
       </c>
-      <c r="M13" s="68"/>
+      <c r="M13" s="94"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
       <c r="P13" s="9"/>
@@ -2069,31 +2073,31 @@
       <c r="A14" s="36"/>
       <c r="B14" s="16"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="90"/>
+      <c r="D14" s="82"/>
       <c r="E14" s="33"/>
       <c r="F14" s="65"/>
-      <c r="G14" s="93"/>
-      <c r="H14" s="96"/>
-      <c r="I14" s="96"/>
-      <c r="J14" s="87"/>
+      <c r="G14" s="85"/>
+      <c r="H14" s="69"/>
+      <c r="I14" s="69"/>
+      <c r="J14" s="92"/>
       <c r="K14" s="65"/>
       <c r="L14" s="11"/>
-      <c r="M14" s="69"/>
+      <c r="M14" s="95"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
       <c r="P14" s="9"/>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="36"/>
-      <c r="F15" s="72" t="str">
+      <c r="F15" s="99" t="str">
         <f>J5</f>
         <v>100mm</v>
       </c>
-      <c r="G15" s="72"/>
-      <c r="H15" s="72"/>
-      <c r="I15" s="72"/>
-      <c r="J15" s="72"/>
-      <c r="K15" s="72"/>
+      <c r="G15" s="99"/>
+      <c r="H15" s="99"/>
+      <c r="I15" s="99"/>
+      <c r="J15" s="99"/>
+      <c r="K15" s="99"/>
       <c r="P15" s="5"/>
     </row>
     <row r="16" spans="1:16" ht="18" thickBot="1">
@@ -2104,22 +2108,22 @@
       <c r="A17" s="36"/>
       <c r="B17" s="16"/>
       <c r="C17" s="3"/>
-      <c r="D17" s="88" t="str">
+      <c r="D17" s="80" t="str">
         <f>B5</f>
         <v>WAGO
 770-173</v>
       </c>
       <c r="E17" s="31"/>
       <c r="F17" s="62"/>
-      <c r="G17" s="91"/>
-      <c r="H17" s="94" t="s">
+      <c r="G17" s="83"/>
+      <c r="H17" s="67" t="s">
         <v>44</v>
       </c>
-      <c r="I17" s="94"/>
-      <c r="J17" s="85"/>
+      <c r="I17" s="67"/>
+      <c r="J17" s="90"/>
       <c r="K17" s="63"/>
       <c r="L17" s="10"/>
-      <c r="M17" s="67" t="str">
+      <c r="M17" s="93" t="str">
         <f>O5</f>
         <v>YEONHO
 YH396-05V</v>
@@ -2132,7 +2136,7 @@
       <c r="A18" s="36"/>
       <c r="B18" s="16"/>
       <c r="C18" s="3"/>
-      <c r="D18" s="89"/>
+      <c r="D18" s="81"/>
       <c r="E18" s="32" t="s">
         <v>28</v>
       </c>
@@ -2140,42 +2144,42 @@
         <f>F5</f>
         <v>L/DC 110V / CON1-Vin+</v>
       </c>
-      <c r="G18" s="92"/>
-      <c r="H18" s="95"/>
-      <c r="I18" s="95"/>
-      <c r="J18" s="86"/>
+      <c r="G18" s="84"/>
+      <c r="H18" s="68"/>
+      <c r="I18" s="68"/>
+      <c r="J18" s="91"/>
       <c r="K18" s="64"/>
       <c r="L18" s="66">
         <v>3</v>
       </c>
-      <c r="M18" s="68"/>
+      <c r="M18" s="94"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
       <c r="P18" s="9"/>
     </row>
     <row r="19" spans="1:17" s="8" customFormat="1" ht="16.5" customHeight="1">
       <c r="A19" s="36"/>
-      <c r="B19" s="70"/>
-      <c r="C19" s="71"/>
-      <c r="D19" s="89"/>
+      <c r="B19" s="100"/>
+      <c r="C19" s="101"/>
+      <c r="D19" s="81"/>
       <c r="E19" s="32"/>
       <c r="F19" s="64"/>
-      <c r="G19" s="92"/>
-      <c r="H19" s="95"/>
-      <c r="I19" s="95"/>
-      <c r="J19" s="86"/>
+      <c r="G19" s="84"/>
+      <c r="H19" s="68"/>
+      <c r="I19" s="68"/>
+      <c r="J19" s="91"/>
       <c r="K19" s="64"/>
       <c r="L19" s="34"/>
-      <c r="M19" s="68"/>
+      <c r="M19" s="94"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
       <c r="P19" s="9"/>
     </row>
     <row r="20" spans="1:17" s="8" customFormat="1" ht="16.5" customHeight="1">
       <c r="A20" s="36"/>
-      <c r="B20" s="70"/>
-      <c r="C20" s="71"/>
-      <c r="D20" s="89"/>
+      <c r="B20" s="100"/>
+      <c r="C20" s="101"/>
+      <c r="D20" s="81"/>
       <c r="E20" s="32" t="s">
         <v>30</v>
       </c>
@@ -2183,15 +2187,15 @@
         <f>F7</f>
         <v>N/DC GND / CON1-Vin-</v>
       </c>
-      <c r="G20" s="92"/>
-      <c r="H20" s="95"/>
-      <c r="I20" s="95"/>
-      <c r="J20" s="86"/>
+      <c r="G20" s="84"/>
+      <c r="H20" s="68"/>
+      <c r="I20" s="68"/>
+      <c r="J20" s="91"/>
       <c r="K20" s="64"/>
       <c r="L20" s="34">
         <v>1</v>
       </c>
-      <c r="M20" s="68"/>
+      <c r="M20" s="94"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
       <c r="P20" s="9"/>
@@ -2200,31 +2204,31 @@
       <c r="A21" s="36"/>
       <c r="B21" s="16"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="90"/>
+      <c r="D21" s="82"/>
       <c r="E21" s="33"/>
       <c r="F21" s="65"/>
-      <c r="G21" s="93"/>
-      <c r="H21" s="96"/>
-      <c r="I21" s="96"/>
-      <c r="J21" s="87"/>
+      <c r="G21" s="85"/>
+      <c r="H21" s="69"/>
+      <c r="I21" s="69"/>
+      <c r="J21" s="92"/>
       <c r="K21" s="65"/>
       <c r="L21" s="11"/>
-      <c r="M21" s="69"/>
+      <c r="M21" s="95"/>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
       <c r="P21" s="9"/>
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="36"/>
-      <c r="F22" s="72" t="str">
+      <c r="F22" s="99" t="str">
         <f>J5</f>
         <v>100mm</v>
       </c>
-      <c r="G22" s="72"/>
-      <c r="H22" s="72"/>
-      <c r="I22" s="72"/>
-      <c r="J22" s="72"/>
-      <c r="K22" s="72"/>
+      <c r="G22" s="99"/>
+      <c r="H22" s="99"/>
+      <c r="I22" s="99"/>
+      <c r="J22" s="99"/>
+      <c r="K22" s="99"/>
       <c r="P22" s="5"/>
     </row>
     <row r="23" spans="1:17">
@@ -2246,27 +2250,27 @@
       <c r="C25" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="75" t="s">
+      <c r="D25" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="75"/>
-      <c r="F25" s="75" t="s">
+      <c r="E25" s="86"/>
+      <c r="F25" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="G25" s="75"/>
-      <c r="H25" s="75"/>
-      <c r="I25" s="75"/>
+      <c r="G25" s="86"/>
+      <c r="H25" s="86"/>
+      <c r="I25" s="86"/>
       <c r="J25" s="29" t="s">
         <v>13</v>
       </c>
       <c r="K25" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="L25" s="75" t="s">
+      <c r="L25" s="86" t="s">
         <v>15</v>
       </c>
-      <c r="M25" s="75"/>
-      <c r="N25" s="75"/>
+      <c r="M25" s="86"/>
+      <c r="N25" s="86"/>
       <c r="O25" s="29" t="s">
         <v>16</v>
       </c>
@@ -2281,27 +2285,27 @@
       <c r="C26" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D26" s="83" t="s">
+      <c r="D26" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="E26" s="83"/>
-      <c r="F26" s="84" t="s">
+      <c r="E26" s="73"/>
+      <c r="F26" s="75" t="s">
         <v>34</v>
       </c>
-      <c r="G26" s="84"/>
-      <c r="H26" s="84"/>
-      <c r="I26" s="84"/>
+      <c r="G26" s="75"/>
+      <c r="H26" s="75"/>
+      <c r="I26" s="75"/>
       <c r="J26" s="25">
         <v>2</v>
       </c>
       <c r="K26" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="L26" s="73" t="s">
+      <c r="L26" s="96" t="s">
         <v>36</v>
       </c>
-      <c r="M26" s="73"/>
-      <c r="N26" s="73"/>
+      <c r="M26" s="96"/>
+      <c r="N26" s="96"/>
       <c r="O26" s="25"/>
       <c r="P26" s="9"/>
     </row>
@@ -2313,27 +2317,27 @@
       <c r="C27" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D27" s="83" t="s">
+      <c r="D27" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="E27" s="83"/>
-      <c r="F27" s="84" t="s">
+      <c r="E27" s="73"/>
+      <c r="F27" s="75" t="s">
         <v>35</v>
       </c>
-      <c r="G27" s="84"/>
-      <c r="H27" s="84"/>
-      <c r="I27" s="84"/>
+      <c r="G27" s="75"/>
+      <c r="H27" s="75"/>
+      <c r="I27" s="75"/>
       <c r="J27" s="25">
         <v>3</v>
       </c>
       <c r="K27" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="L27" s="73" t="s">
+      <c r="L27" s="96" t="s">
         <v>38</v>
       </c>
-      <c r="M27" s="73"/>
-      <c r="N27" s="73"/>
+      <c r="M27" s="96"/>
+      <c r="N27" s="96"/>
       <c r="O27" s="25"/>
       <c r="P27" s="9"/>
     </row>
@@ -2345,25 +2349,25 @@
       <c r="C28" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D28" s="83" t="s">
+      <c r="D28" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="E28" s="83"/>
-      <c r="F28" s="84"/>
-      <c r="G28" s="84"/>
-      <c r="H28" s="84"/>
-      <c r="I28" s="84"/>
+      <c r="E28" s="73"/>
+      <c r="F28" s="75"/>
+      <c r="G28" s="75"/>
+      <c r="H28" s="75"/>
+      <c r="I28" s="75"/>
       <c r="J28" s="26">
         <v>6</v>
       </c>
       <c r="K28" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="L28" s="83" t="s">
+      <c r="L28" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="M28" s="83"/>
-      <c r="N28" s="83"/>
+      <c r="M28" s="73"/>
+      <c r="N28" s="73"/>
       <c r="O28" s="26"/>
       <c r="P28" s="22"/>
     </row>
@@ -2375,32 +2379,32 @@
       <c r="C29" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="D29" s="83"/>
-      <c r="E29" s="83"/>
-      <c r="F29" s="84"/>
-      <c r="G29" s="84"/>
-      <c r="H29" s="84"/>
-      <c r="I29" s="84"/>
+      <c r="D29" s="73"/>
+      <c r="E29" s="73"/>
+      <c r="F29" s="75"/>
+      <c r="G29" s="75"/>
+      <c r="H29" s="75"/>
+      <c r="I29" s="75"/>
       <c r="J29" s="26"/>
       <c r="K29" s="26"/>
-      <c r="L29" s="83"/>
-      <c r="M29" s="83"/>
-      <c r="N29" s="83"/>
+      <c r="L29" s="73"/>
+      <c r="M29" s="73"/>
+      <c r="N29" s="73"/>
       <c r="O29" s="26"/>
       <c r="P29" s="22"/>
     </row>
     <row r="30" spans="1:17" s="21" customFormat="1" ht="25" customHeight="1">
       <c r="A30" s="42"/>
-      <c r="B30" s="100" t="s">
+      <c r="B30" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="101"/>
-      <c r="D30" s="101"/>
-      <c r="E30" s="101"/>
-      <c r="F30" s="101"/>
-      <c r="G30" s="101"/>
-      <c r="H30" s="101"/>
-      <c r="I30" s="102"/>
+      <c r="C30" s="78"/>
+      <c r="D30" s="78"/>
+      <c r="E30" s="78"/>
+      <c r="F30" s="78"/>
+      <c r="G30" s="78"/>
+      <c r="H30" s="78"/>
+      <c r="I30" s="79"/>
       <c r="J30" s="19"/>
       <c r="K30" s="45"/>
       <c r="L30" s="45"/>
@@ -2463,18 +2467,18 @@
       <c r="C34" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="D34" s="79" t="s">
+      <c r="D34" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="E34" s="79"/>
-      <c r="F34" s="79"/>
-      <c r="G34" s="79"/>
-      <c r="H34" s="79"/>
-      <c r="I34" s="79"/>
-      <c r="J34" s="79" t="s">
+      <c r="E34" s="76"/>
+      <c r="F34" s="76"/>
+      <c r="G34" s="76"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="76"/>
+      <c r="J34" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="K34" s="79"/>
+      <c r="K34" s="76"/>
       <c r="P34" s="9"/>
     </row>
     <row r="35" spans="1:16">
@@ -2485,16 +2489,16 @@
       <c r="C35" s="27">
         <v>45486</v>
       </c>
-      <c r="D35" s="97" t="s">
+      <c r="D35" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="E35" s="97"/>
-      <c r="F35" s="97"/>
-      <c r="G35" s="97"/>
-      <c r="H35" s="97"/>
-      <c r="I35" s="97"/>
-      <c r="J35" s="98"/>
-      <c r="K35" s="98"/>
+      <c r="E35" s="74"/>
+      <c r="F35" s="74"/>
+      <c r="G35" s="74"/>
+      <c r="H35" s="74"/>
+      <c r="I35" s="74"/>
+      <c r="J35" s="71"/>
+      <c r="K35" s="71"/>
       <c r="P35" s="9"/>
     </row>
     <row r="36" spans="1:16">
@@ -2505,60 +2509,60 @@
       <c r="C36" s="27">
         <v>45497</v>
       </c>
-      <c r="D36" s="104" t="s">
+      <c r="D36" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="E36" s="104"/>
-      <c r="F36" s="104"/>
-      <c r="G36" s="104"/>
-      <c r="H36" s="104"/>
-      <c r="I36" s="104"/>
-      <c r="J36" s="98" t="s">
+      <c r="E36" s="70"/>
+      <c r="F36" s="70"/>
+      <c r="G36" s="70"/>
+      <c r="H36" s="70"/>
+      <c r="I36" s="70"/>
+      <c r="J36" s="71" t="s">
         <v>47</v>
       </c>
-      <c r="K36" s="98"/>
+      <c r="K36" s="71"/>
       <c r="P36" s="9"/>
     </row>
     <row r="37" spans="1:16">
       <c r="A37" s="56"/>
       <c r="B37" s="26"/>
       <c r="C37" s="27"/>
-      <c r="D37" s="97"/>
-      <c r="E37" s="97"/>
-      <c r="F37" s="97"/>
-      <c r="G37" s="97"/>
-      <c r="H37" s="97"/>
-      <c r="I37" s="97"/>
-      <c r="J37" s="98"/>
-      <c r="K37" s="98"/>
+      <c r="D37" s="74"/>
+      <c r="E37" s="74"/>
+      <c r="F37" s="74"/>
+      <c r="G37" s="74"/>
+      <c r="H37" s="74"/>
+      <c r="I37" s="74"/>
+      <c r="J37" s="71"/>
+      <c r="K37" s="71"/>
       <c r="P37" s="9"/>
     </row>
     <row r="38" spans="1:16">
       <c r="A38" s="56"/>
       <c r="B38" s="26"/>
       <c r="C38" s="27"/>
-      <c r="D38" s="97"/>
-      <c r="E38" s="97"/>
-      <c r="F38" s="97"/>
-      <c r="G38" s="97"/>
-      <c r="H38" s="97"/>
-      <c r="I38" s="97"/>
-      <c r="J38" s="98"/>
-      <c r="K38" s="98"/>
+      <c r="D38" s="74"/>
+      <c r="E38" s="74"/>
+      <c r="F38" s="74"/>
+      <c r="G38" s="74"/>
+      <c r="H38" s="74"/>
+      <c r="I38" s="74"/>
+      <c r="J38" s="71"/>
+      <c r="K38" s="71"/>
       <c r="P38" s="9"/>
     </row>
     <row r="39" spans="1:16">
       <c r="A39" s="56"/>
       <c r="B39" s="26"/>
       <c r="C39" s="28"/>
-      <c r="D39" s="97"/>
-      <c r="E39" s="97"/>
-      <c r="F39" s="97"/>
-      <c r="G39" s="97"/>
-      <c r="H39" s="97"/>
-      <c r="I39" s="97"/>
-      <c r="J39" s="98"/>
-      <c r="K39" s="98"/>
+      <c r="D39" s="74"/>
+      <c r="E39" s="74"/>
+      <c r="F39" s="74"/>
+      <c r="G39" s="74"/>
+      <c r="H39" s="74"/>
+      <c r="I39" s="74"/>
+      <c r="J39" s="71"/>
+      <c r="K39" s="71"/>
       <c r="P39" s="9"/>
     </row>
     <row r="40" spans="1:16">
@@ -2591,13 +2595,45 @@
       <c r="O41" s="14"/>
       <c r="P41" s="15"/>
     </row>
+    <row r="43" spans="1:16" ht="30">
+      <c r="L43" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="H10:I14"/>
-    <mergeCell ref="D36:I36"/>
-    <mergeCell ref="J36:K36"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="M17:M21"/>
+    <mergeCell ref="B19:C20"/>
+    <mergeCell ref="F22:K22"/>
+    <mergeCell ref="L27:N27"/>
+    <mergeCell ref="B1:O1"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="N5:N7"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="J10:J14"/>
+    <mergeCell ref="J17:J21"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="M10:M14"/>
+    <mergeCell ref="L25:N25"/>
+    <mergeCell ref="L26:N26"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="F15:K15"/>
+    <mergeCell ref="B12:C13"/>
+    <mergeCell ref="D10:D14"/>
+    <mergeCell ref="G10:G14"/>
     <mergeCell ref="L28:N28"/>
     <mergeCell ref="D39:I39"/>
     <mergeCell ref="J39:K39"/>
@@ -2614,6 +2650,11 @@
     <mergeCell ref="J34:K34"/>
     <mergeCell ref="B30:I30"/>
     <mergeCell ref="D28:E28"/>
+    <mergeCell ref="H10:I14"/>
+    <mergeCell ref="D36:I36"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D27:E27"/>
     <mergeCell ref="F28:I28"/>
     <mergeCell ref="F27:I27"/>
     <mergeCell ref="D17:D21"/>
@@ -2621,38 +2662,6 @@
     <mergeCell ref="H17:I21"/>
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="F25:I25"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="J10:J14"/>
-    <mergeCell ref="J17:J21"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="M10:M14"/>
-    <mergeCell ref="L25:N25"/>
-    <mergeCell ref="L26:N26"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="F15:K15"/>
-    <mergeCell ref="B12:C13"/>
-    <mergeCell ref="D10:D14"/>
-    <mergeCell ref="G10:G14"/>
-    <mergeCell ref="M17:M21"/>
-    <mergeCell ref="B19:C20"/>
-    <mergeCell ref="F22:K22"/>
-    <mergeCell ref="L27:N27"/>
-    <mergeCell ref="B1:O1"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="N5:N7"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="D6:E6"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>